<commit_message>
added project idea to the list
</commit_message>
<xml_diff>
--- a/Logs.xlsx
+++ b/Logs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xGino/GitHub/PERSONAL/xgino/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E159B5-3DB9-0C48-A034-AB1747FC49E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CFEA2FE-2150-AB46-B361-B0B64F88F7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="15700" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="88">
   <si>
     <t>Date</t>
   </si>
@@ -260,6 +260,48 @@
   </si>
   <si>
     <t>Check Verkoop prognose Fix mail add promotie</t>
+  </si>
+  <si>
+    <t>check voeg speler toe, maar server error 500, fix in code next time</t>
+  </si>
+  <si>
+    <t>Create message</t>
+  </si>
+  <si>
+    <t>Message to mohsen</t>
+  </si>
+  <si>
+    <t>Fix Personal Github MAC</t>
+  </si>
+  <si>
+    <t>Mac Github</t>
+  </si>
+  <si>
+    <t>Hockey Stick zoeken</t>
+  </si>
+  <si>
+    <t>Hockey</t>
+  </si>
+  <si>
+    <t>QR Dive Mail</t>
+  </si>
+  <si>
+    <t>QR dive mail fix end in spam | Only work for gmail not outlook</t>
+  </si>
+  <si>
+    <t>make project planning for xgino data science projects</t>
+  </si>
+  <si>
+    <t>Xgino project</t>
+  </si>
+  <si>
+    <t>Clean up QR dive todo items and prioritize them</t>
+  </si>
+  <si>
+    <t>QR Dive todo</t>
+  </si>
+  <si>
+    <t>FOOD</t>
   </si>
 </sst>
 </file>
@@ -824,7 +866,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -842,11 +884,11 @@
       </c>
       <c r="C1" s="7">
         <f ca="1">SUMIFS(TODO!J:J,TODO!B:B,TODAY())</f>
-        <v>4.1666666666666741E-2</v>
+        <v>0.12499999999999994</v>
       </c>
       <c r="D1" s="8">
         <f ca="1">C1*24</f>
-        <v>1.0000000000000018</v>
+        <v>2.9999999999999987</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -869,7 +911,7 @@
       </c>
       <c r="C4" s="7">
         <f>SUMIFS(TODO!J:J, TODO!B:B, "&gt;="&amp;DATE($A1, MONTH(DATEVALUE(C$3 &amp; " 1")), 1), TODO!B:B, "&lt;="&amp;EOMONTH(DATE($A1, MONTH(DATEVALUE(C$3 &amp; " 1")), 1), 0))</f>
-        <v>1.0416666666666665</v>
+        <v>1.3749999999999998</v>
       </c>
       <c r="D4" s="7">
         <f>SUMIFS(TODO!K:K, TODO!C:C, "&gt;="&amp;DATE($A1, MONTH(DATEVALUE(D$3 &amp; " 1")), 1), TODO!C:C, "&lt;="&amp;EOMONTH(DATE($A1, MONTH(DATEVALUE(D$3 &amp; " 1")), 1), 0))</f>
@@ -886,7 +928,7 @@
       </c>
       <c r="C5" s="7">
         <f t="shared" ref="C5:E6" si="0">C4/4</f>
-        <v>0.26041666666666663</v>
+        <v>0.34374999999999994</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="0"/>
@@ -903,7 +945,7 @@
       </c>
       <c r="C6" s="7">
         <f t="shared" si="0"/>
-        <v>6.5104166666666657E-2</v>
+        <v>8.5937499999999986E-2</v>
       </c>
       <c r="D6" s="7">
         <f t="shared" si="0"/>
@@ -920,7 +962,7 @@
       </c>
       <c r="C8" s="7">
         <f>SUMIFS(TODO!J:J, TODO!C:C, "Univercity", TODO!B:B, "&gt;=" &amp; DATE($A1, MONTH(DATEVALUE(C$3 &amp; " 1")), 1), TODO!B:B, "&lt;=" &amp; EOMONTH(DATE($A1, MONTH(DATEVALUE(C$3 &amp; " 1")), 1), 0))</f>
-        <v>8.3333333333333259E-2</v>
+        <v>9.3749999999999889E-2</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
@@ -931,7 +973,7 @@
       </c>
       <c r="C9" s="7">
         <f t="shared" ref="C9:E10" si="1">C8/4</f>
-        <v>2.0833333333333315E-2</v>
+        <v>2.3437499999999972E-2</v>
       </c>
       <c r="D9" s="7">
         <f t="shared" si="1"/>
@@ -948,7 +990,7 @@
       </c>
       <c r="C10" s="7">
         <f t="shared" si="1"/>
-        <v>5.2083333333333287E-3</v>
+        <v>5.8593749999999931E-3</v>
       </c>
       <c r="D10" s="7">
         <f t="shared" si="1"/>
@@ -975,7 +1017,7 @@
       </c>
       <c r="C13" s="7">
         <f>SUMIFS(TODO!J:J, TODO!C:C, "E Commerce", TODO!B:B, "&gt;=" &amp; DATE($A1, MONTH(DATEVALUE(C$3 &amp; " 1")), 1), TODO!B:B, "&lt;=" &amp; EOMONTH(DATE($A1, MONTH(DATEVALUE(C$3 &amp; " 1")), 1), 0))</f>
-        <v>0.21875</v>
+        <v>0.26041666666666663</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -986,7 +1028,7 @@
       </c>
       <c r="C14" s="7">
         <f t="shared" ref="C14:E15" si="2">C13/4</f>
-        <v>5.46875E-2</v>
+        <v>6.5104166666666657E-2</v>
       </c>
       <c r="D14" s="7">
         <f t="shared" si="2"/>
@@ -1003,7 +1045,7 @@
       </c>
       <c r="C15" s="7">
         <f t="shared" si="2"/>
-        <v>1.3671875E-2</v>
+        <v>1.6276041666666664E-2</v>
       </c>
       <c r="D15" s="7">
         <f t="shared" si="2"/>
@@ -1030,7 +1072,7 @@
       </c>
       <c r="C18" s="7">
         <f>SUMIFS(TODO!J:J, TODO!C:C, "SaaS", TODO!B:B, "&gt;=" &amp; DATE($A1, MONTH(DATEVALUE(C$3 &amp; " 1")), 1), TODO!B:B, "&lt;=" &amp; EOMONTH(DATE($A1, MONTH(DATEVALUE(C$3 &amp; " 1")), 1), 0))</f>
-        <v>0.25</v>
+        <v>0.37499999999999994</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
@@ -1042,7 +1084,7 @@
       </c>
       <c r="C19" s="7">
         <f t="shared" ref="C19:E20" si="3">C18/4</f>
-        <v>6.25E-2</v>
+        <v>9.3749999999999986E-2</v>
       </c>
       <c r="D19" s="7">
         <f t="shared" si="3"/>
@@ -1060,7 +1102,7 @@
       </c>
       <c r="C20" s="7">
         <f t="shared" si="3"/>
-        <v>1.5625E-2</v>
+        <v>2.3437499999999997E-2</v>
       </c>
       <c r="D20" s="7">
         <f t="shared" si="3"/>
@@ -1146,7 +1188,7 @@
       </c>
       <c r="C28" s="7">
         <f>SUMIFS(TODO!J:J, TODO!C:C, "Project", TODO!B:B, "&gt;=" &amp; DATE($A1, MONTH(DATEVALUE(C$3 &amp; " 1")), 1), TODO!B:B, "&lt;=" &amp; EOMONTH(DATE($A1, MONTH(DATEVALUE(C$3 &amp; " 1")), 1), 0))</f>
-        <v>0.23958333333333326</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -1157,7 +1199,7 @@
       </c>
       <c r="C29" s="7">
         <f t="shared" ref="C29:E30" si="5">C28/4</f>
-        <v>5.9895833333333315E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D29" s="7">
         <f t="shared" si="5"/>
@@ -1174,7 +1216,7 @@
       </c>
       <c r="C30" s="7">
         <f t="shared" si="5"/>
-        <v>1.4973958333333329E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="D30" s="7">
         <f t="shared" si="5"/>
@@ -1197,10 +1239,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:M21"/>
+  <dimension ref="B1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.25"/>
@@ -1583,7 +1625,7 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="J14" s="16">
-        <f t="shared" ref="J14:J21" si="1">IF(I14 &lt; H14, I14 + 1, I14) - H14</f>
+        <f t="shared" ref="J14:J29" si="1">IF(I14 &lt; H14, I14 + 1, I14) - H14</f>
         <v>2.083333333333337E-2</v>
       </c>
     </row>
@@ -1769,14 +1811,224 @@
         <v>24</v>
       </c>
       <c r="H21" s="16">
-        <v>0.60416666666666663</v>
+        <v>0.5625</v>
       </c>
       <c r="I21" s="16">
         <v>0.64583333333333337</v>
       </c>
       <c r="J21" s="16">
         <f t="shared" si="1"/>
-        <v>4.1666666666666741E-2</v>
+        <v>8.333333333333337E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="34" x14ac:dyDescent="0.25">
+      <c r="B22" s="21">
+        <v>45580</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="16">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I22" s="16">
+        <v>0.65625</v>
+      </c>
+      <c r="J22" s="16">
+        <f t="shared" si="1"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="17" x14ac:dyDescent="0.25">
+      <c r="B23" s="21">
+        <v>45580</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" s="16">
+        <v>0.65625</v>
+      </c>
+      <c r="I23" s="16">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J23" s="16">
+        <f t="shared" si="1"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="21">
+        <v>45580</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="16">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I24" s="16">
+        <v>0.6875</v>
+      </c>
+      <c r="J24" s="16">
+        <f t="shared" si="1"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="17" x14ac:dyDescent="0.25">
+      <c r="B25" s="21">
+        <v>45580</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" s="16">
+        <v>0.6875</v>
+      </c>
+      <c r="I25" s="16">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="J25" s="16">
+        <f t="shared" si="1"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" ht="34" x14ac:dyDescent="0.25">
+      <c r="B26" s="21">
+        <v>45580</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="16">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="I26" s="16">
+        <v>0.8125</v>
+      </c>
+      <c r="J26" s="16">
+        <f t="shared" si="1"/>
+        <v>0.10416666666666663</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="17" x14ac:dyDescent="0.25">
+      <c r="B27" s="21">
+        <v>45581</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" s="16">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I27" s="16">
+        <v>0.46875</v>
+      </c>
+      <c r="J27" s="16">
+        <f t="shared" si="1"/>
+        <v>5.2083333333333315E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" ht="17" x14ac:dyDescent="0.25">
+      <c r="B28" s="21">
+        <v>45581</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" s="16">
+        <v>0.46875</v>
+      </c>
+      <c r="I28" s="16">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="J28" s="16">
+        <f t="shared" si="1"/>
+        <v>2.0833333333333315E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="17" x14ac:dyDescent="0.25">
+      <c r="B29" s="21">
+        <v>45581</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29" s="16">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="I29" s="16">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="J29" s="16">
+        <f t="shared" si="1"/>
+        <v>5.2083333333333315E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1816,7 +2068,7 @@
           <x14:formula1>
             <xm:f>Category!$D$3:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>G3:G8 G10:G11 G13:G21</xm:sqref>
+          <xm:sqref>G3:G8 G10:G11 G13:G29</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6015FAEB-E6D3-49C6-8FAB-F4CAAB2DF346}">
           <x14:formula1>

</xml_diff>